<commit_message>
Pago de obligaciones version beta
</commit_message>
<xml_diff>
--- a/MercuryTours/Resources/datapool/cupones.xlsx
+++ b/MercuryTours/Resources/datapool/cupones.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="4770"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>nit empresa</t>
   </si>
@@ -184,34 +185,28 @@
     <t>102153</t>
   </si>
   <si>
-    <t>4665498641489</t>
-  </si>
-  <si>
-    <t>04408894094</t>
-  </si>
-  <si>
-    <t>09498984894</t>
-  </si>
-  <si>
-    <t>894894944</t>
-  </si>
-  <si>
-    <t>4894894184</t>
-  </si>
-  <si>
-    <t>848496441</t>
-  </si>
-  <si>
-    <t>48946948984</t>
-  </si>
-  <si>
-    <t>48949848</t>
-  </si>
-  <si>
-    <t>4984988497</t>
-  </si>
-  <si>
-    <t>4894894948989</t>
+    <t>4157707229253257802023752304390000015702209620171030</t>
+  </si>
+  <si>
+    <t>4157707229253257802023752304390000005702209620171030</t>
+  </si>
+  <si>
+    <t>4157707229253257802023752304390000000702209620171030</t>
+  </si>
+  <si>
+    <t>4157707229253257802023752304390000000552209620171030</t>
+  </si>
+  <si>
+    <t>41577072292532578020237523043900000008802209620171030</t>
+  </si>
+  <si>
+    <t>4157707229253257802023752304390000005712209620171030</t>
+  </si>
+  <si>
+    <t>415770722925325780202375230439000007702209620171030</t>
+  </si>
+  <si>
+    <t>4157707229253257802023752304390000008702209620171030</t>
   </si>
 </sst>
 </file>
@@ -563,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K7"/>
+  <dimension ref="A2:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +570,7 @@
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -610,7 +605,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -645,7 +640,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -680,7 +675,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -715,15 +710,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>58</v>
@@ -732,25 +727,37 @@
         <v>59</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>65</v>
+      <c r="L6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>